<commit_message>
cambia algunos datos para pruebas
</commit_message>
<xml_diff>
--- a/Envio de WhatsApp/Numero_mensaje_whatsapp.xlsx
+++ b/Envio de WhatsApp/Numero_mensaje_whatsapp.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\proyectos empresa\IMGWHATS\Envio de WhatsApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\WhappClone\IMGWHATS\Envio de WhatsApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7620"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="20460" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Cod</t>
   </si>
@@ -44,112 +44,40 @@
     <t>Valor factura</t>
   </si>
   <si>
-    <t>Derwin</t>
-  </si>
-  <si>
-    <t>Ferrevidrio Raul</t>
-  </si>
-  <si>
-    <t>168800.00</t>
-  </si>
-  <si>
-    <t>Ferrelectricos el Brillante</t>
-  </si>
-  <si>
-    <t>102150.00</t>
-  </si>
-  <si>
-    <t>Ferreteria JGB</t>
-  </si>
-  <si>
-    <t>274550.00</t>
-  </si>
-  <si>
-    <t>Ferreteria GYY</t>
-  </si>
-  <si>
-    <t>263600.00</t>
-  </si>
-  <si>
-    <t>Ferreteria Ecoferr</t>
-  </si>
-  <si>
-    <t>539775.00</t>
-  </si>
-  <si>
-    <t>Ferrelectricos mundial</t>
-  </si>
-  <si>
-    <t>101250.00</t>
-  </si>
-  <si>
-    <t>Ferrelecto</t>
-  </si>
-  <si>
-    <t>323454.00</t>
-  </si>
-  <si>
-    <t>546</t>
-  </si>
-  <si>
-    <t>183</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>211</t>
-  </si>
-  <si>
-    <t>74</t>
-  </si>
-  <si>
-    <t>149</t>
-  </si>
-  <si>
-    <t>535</t>
-  </si>
-  <si>
-    <t>3128026914</t>
-  </si>
-  <si>
-    <t>3213616393</t>
-  </si>
-  <si>
-    <t>3118807384</t>
-  </si>
-  <si>
-    <t>3144277255</t>
-  </si>
-  <si>
-    <t>3114438952</t>
-  </si>
-  <si>
-    <t>3222060300</t>
-  </si>
-  <si>
-    <t>3026477698</t>
-  </si>
-  <si>
-    <t>7890</t>
-  </si>
-  <si>
-    <t>7891</t>
-  </si>
-  <si>
-    <t>7893</t>
-  </si>
-  <si>
-    <t>7894</t>
-  </si>
-  <si>
-    <t>7895</t>
-  </si>
-  <si>
-    <t>7897</t>
-  </si>
-  <si>
-    <t>7902</t>
+    <t>777</t>
+  </si>
+  <si>
+    <t>Ferreteria Marley</t>
+  </si>
+  <si>
+    <t>Gerson</t>
+  </si>
+  <si>
+    <t>Jesus Andres</t>
+  </si>
+  <si>
+    <t>3219155489</t>
+  </si>
+  <si>
+    <t>12000</t>
+  </si>
+  <si>
+    <t>7777</t>
+  </si>
+  <si>
+    <t>794</t>
+  </si>
+  <si>
+    <t>Ferreteria jsjs</t>
+  </si>
+  <si>
+    <t>3187686326</t>
+  </si>
+  <si>
+    <t>20000</t>
+  </si>
+  <si>
+    <t>7942</t>
   </si>
 </sst>
 </file>
@@ -491,7 +419,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,143 +451,73 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>37</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="A5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>40</v>
-      </c>
+      <c r="A7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="A8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Se Cambian paths y metodos
Se cambió el método para encontrar y seleccionar contacto, se cambia el xpath para cerrar sesión
</commit_message>
<xml_diff>
--- a/Envio de WhatsApp/Numero_mensaje_whatsapp.xlsx
+++ b/Envio de WhatsApp/Numero_mensaje_whatsapp.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="20460" windowHeight="7620"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="20460" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Cod</t>
   </si>
@@ -78,6 +79,54 @@
   </si>
   <si>
     <t>7942</t>
+  </si>
+  <si>
+    <t>666</t>
+  </si>
+  <si>
+    <t>Ferreteria 1</t>
+  </si>
+  <si>
+    <t>sebas</t>
+  </si>
+  <si>
+    <t>3227804602</t>
+  </si>
+  <si>
+    <t>121212</t>
+  </si>
+  <si>
+    <t>1111</t>
+  </si>
+  <si>
+    <t>555</t>
+  </si>
+  <si>
+    <t>Ferreteria 2</t>
+  </si>
+  <si>
+    <t>Melqui</t>
+  </si>
+  <si>
+    <t>2222</t>
+  </si>
+  <si>
+    <t>3176794454</t>
+  </si>
+  <si>
+    <t>1212</t>
+  </si>
+  <si>
+    <t>asdasdfv</t>
+  </si>
+  <si>
+    <t>4545454545</t>
+  </si>
+  <si>
+    <t>3333</t>
+  </si>
+  <si>
+    <t>imagine</t>
   </si>
 </sst>
 </file>
@@ -419,7 +468,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,22 +539,64 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>

</xml_diff>

<commit_message>
Actualización de manejo XL
</commit_message>
<xml_diff>
--- a/Envio de WhatsApp/Numero_mensaje_whatsapp.xlsx
+++ b/Envio de WhatsApp/Numero_mensaje_whatsapp.xlsx
@@ -9,13 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="20460" windowHeight="7620"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="20460" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -468,7 +467,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Generalización de manejo XL
parte 2 de la generalizacion de manejo XL
</commit_message>
<xml_diff>
--- a/Envio de WhatsApp/Numero_mensaje_whatsapp.xlsx
+++ b/Envio de WhatsApp/Numero_mensaje_whatsapp.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Documents\WhappClone\IMGWHATS\Envio de WhatsApp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PROGRAMACION\pythonxD\IMGWHATS\Envio de WhatsApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79AA0CBC-48DA-4142-A86D-FB271AA18F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="20460" windowHeight="7620"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="20910" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>Cod</t>
   </si>
@@ -126,12 +127,30 @@
   </si>
   <si>
     <t>imagine</t>
+  </si>
+  <si>
+    <t>Ferreteria 3</t>
+  </si>
+  <si>
+    <t>imagine2</t>
+  </si>
+  <si>
+    <t>4545</t>
+  </si>
+  <si>
+    <t>xD</t>
+  </si>
+  <si>
+    <t>212121</t>
+  </si>
+  <si>
+    <t>2121</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -463,11 +482,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,16 +617,44 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>